<commit_message>
Commiting changes for application merge attributes
</commit_message>
<xml_diff>
--- a/FolderCorrectionUtility/ProjectDetailsReport.xlsx
+++ b/FolderCorrectionUtility/ProjectDetailsReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\FolderCorrectionUtility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\Conti_AM\FolderCorrectionUtility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B05FC4-96CC-4FB6-A5C7-A0EC80B66BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6E505A-0B23-48B8-A248-8EFC338D679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$1:$F$172</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet0!$A$1:$F$178</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="377">
   <si>
     <t>Project Name</t>
   </si>
@@ -187,6 +187,12 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_xmizkKBJEeybb5qGPqhBnw</t>
   </si>
   <si>
+    <t>ADAS_PG_SYS_ETM_Playground_RM</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_zpnWECqXEe21E5_Yq1_zqA</t>
+  </si>
+  <si>
     <t>WeatherStation_RM_VM_Training_20210930_AM</t>
   </si>
   <si>
@@ -313,6 +319,12 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_wAktcP6SEeyElJh91aOrbw</t>
   </si>
   <si>
+    <t>WeatherStation_RM_VM_HEP_JumpStartTraining_20220921</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_cxMZwDlyEe2_EeET0BmN6Q</t>
+  </si>
+  <si>
     <t>WeatherStationSystems_L1_RM_Generic</t>
   </si>
   <si>
@@ -457,6 +469,12 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_SVBioHL9Eeybb5qGPqhBnw</t>
   </si>
   <si>
+    <t>WeatherStation_RM_VM_HEP_Training_20220909</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_j9ZNMDAbEe21E5_Yq1_zqA</t>
+  </si>
+  <si>
     <t>ADAS_PG_GC_Training_mainConfiguratiion_workon_release1</t>
   </si>
   <si>
@@ -523,6 +541,12 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_02dRYKtbEeybb5qGPqhBnw</t>
   </si>
   <si>
+    <t>ADAS_PG_SYS_RM_JumpStart</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_z-ZSkB97Ee21E5_Yq1_zqA</t>
+  </si>
+  <si>
     <t>WeatherStation_RM_VM_TCI_Demo</t>
   </si>
   <si>
@@ -727,18 +751,24 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_iAAQUCBUEeyKdKtH2BZffQ</t>
   </si>
   <si>
+    <t>ULM_20220909151048</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_kA-MADAjEe21E5_Yq1_zqA</t>
+  </si>
+  <si>
+    <t>WeatherStation_RM_VM_TCI_Demo_HB</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_MxkFgMd9Eeybb5qGPqhBnw</t>
+  </si>
+  <si>
     <t>WeatherStation_RM_VM_HEP_Training_20220113_OR</t>
   </si>
   <si>
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_HTJwoHL9Eeybb5qGPqhBnw</t>
   </si>
   <si>
-    <t>WeatherStation_RM_VM_TCI_Demo_HB</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_MxkFgMd9Eeybb5qGPqhBnw</t>
-  </si>
-  <si>
     <t>ULM_20220708131726</t>
   </si>
   <si>
@@ -829,6 +859,12 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_bVIGUIpYEeybb5qGPqhBnw</t>
   </si>
   <si>
+    <t>WeatherStation_RM_VM_HEP_Harshita</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_NtlloCUDEe21E5_Yq1_zqA</t>
+  </si>
+  <si>
     <t>WeatherStation_RM_VM_Training_20220127_AM_BLR_20220127152755</t>
   </si>
   <si>
@@ -847,6 +883,12 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_5YRzIF2xEeybb5qGPqhBnw</t>
   </si>
   <si>
+    <t>JumpStart_Training_Frankfurt_20220921133045</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_ilHQcDmDEe2_EeET0BmN6Q</t>
+  </si>
+  <si>
     <t>ADAS_PG_SYS_RM_GC_Advanced</t>
   </si>
   <si>
@@ -871,6 +913,12 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_bTdqwHOhEeybb5qGPqhBnw</t>
   </si>
   <si>
+    <t>WeatherStation_RM_VM_HEP_Training_Test08092022</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/__kMdQC9vEe21E5_Yq1_zqA</t>
+  </si>
+  <si>
     <t>BLR_20220429113049</t>
   </si>
   <si>
@@ -901,24 +949,6 @@
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_VOe_EKtQEeybb5qGPqhBnw</t>
   </si>
   <si>
-    <t>test component Initial Stream</t>
-  </si>
-  <si>
-    <t>test component</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/component/_ouV2YA8vEe21E5_Yq1_zqA</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_ousbtg8vEe21E5_Yq1_zqA</t>
-  </si>
-  <si>
-    <t>test stream 1</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_1qb5YA8vEe21E5_Yq1_zqA</t>
-  </si>
-  <si>
     <t>ADAS_PG_SW_RM</t>
   </si>
   <si>
@@ -1030,69 +1060,69 @@
     <t>ADAS_PG_SYS_DesignAM</t>
   </si>
   <si>
+    <t>ADAS_PG_SYS_DesignAM new2</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/component/_IkWrwAQNEeyeAcxn6FaqRw</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_rpNS8JVHEeybb5qGPqhBnw</t>
+  </si>
+  <si>
+    <t>ADAS_PG_SYS_Design_AM_Project_ARS620TA16</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_WY5JIIqVEeybb5qGPqhBnw</t>
+  </si>
+  <si>
+    <t>ADAS_PG_SYS_DesignAM_RMM_Training</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_D3orsBoLEeyaXMo7EM4AOg</t>
+  </si>
+  <si>
+    <t>ADAS_PG_SYS_DesignAM_GC_training</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_ym41kBY5EeyaXMo7EM4AOg</t>
+  </si>
+  <si>
+    <t>ADAS_PG_SYS_DesignAM Test_CRYSTAL_WorkOn</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_9HmbkJY7Eeybb5qGPqhBnw</t>
+  </si>
+  <si>
+    <t>Radar_SYS_Design_AM_PlatformVariant_SSR620</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_oneoIKFMEeybb5qGPqhBnw</t>
+  </si>
+  <si>
+    <t>ADAS_PG_SYS_DesignAM new</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_aB8hUJVHEeybb5qGPqhBnw</t>
+  </si>
+  <si>
+    <t>ADAS_PG_SYS_Design_AM_PlatformVariant_ADC520</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_fy7y8HIxEeybb5qGPqhBnw</t>
+  </si>
+  <si>
+    <t>ADAS_PG_SYS_DesignAM newest</t>
+  </si>
+  <si>
+    <t>https://jazz-test6.conti.de/rm4/cm/stream/_5WWYYJVHEeybb5qGPqhBnw</t>
+  </si>
+  <si>
     <t>ADAS_PG_SYS_DesignAM_Generic</t>
   </si>
   <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/component/_IkWrwAQNEeyeAcxn6FaqRw</t>
-  </si>
-  <si>
     <t>https://jazz-test6.conti.de/rm4/cm/stream/_Ika9NgQNEeyeAcxn6FaqRw</t>
   </si>
   <si>
-    <t>ADAS_PG_SYS_DesignAM Test_CRYSTAL_WorkOn</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_9HmbkJY7Eeybb5qGPqhBnw</t>
-  </si>
-  <si>
-    <t>ADAS_PG_SYS_DesignAM new</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_aB8hUJVHEeybb5qGPqhBnw</t>
-  </si>
-  <si>
-    <t>ADAS_PG_SYS_DesignAM_GC_training</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_ym41kBY5EeyaXMo7EM4AOg</t>
-  </si>
-  <si>
-    <t>ADAS_PG_SYS_Design_AM_Project_ARS620TA16</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_WY5JIIqVEeybb5qGPqhBnw</t>
-  </si>
-  <si>
-    <t>ADAS_PG_SYS_DesignAM newest</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_5WWYYJVHEeybb5qGPqhBnw</t>
-  </si>
-  <si>
-    <t>ADAS_PG_SYS_Design_AM_PlatformVariant_ADC520</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_fy7y8HIxEeybb5qGPqhBnw</t>
-  </si>
-  <si>
-    <t>ADAS_PG_SYS_DesignAM new2</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_rpNS8JVHEeybb5qGPqhBnw</t>
-  </si>
-  <si>
-    <t>Radar_SYS_Design_AM_PlatformVariant_SSR620</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_oneoIKFMEeybb5qGPqhBnw</t>
-  </si>
-  <si>
-    <t>ADAS_PG_SYS_DesignAM_RMM_Training</t>
-  </si>
-  <si>
-    <t>https://jazz-test6.conti.de/rm4/cm/stream/_D3orsBoLEeyaXMo7EM4AOg</t>
-  </si>
-  <si>
     <t>Template_ProjectArea_BU4_AM_V2</t>
   </si>
   <si>
@@ -1124,16 +1154,13 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1145,14 +1172,6 @@
       <b/>
       <sz val="15"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1177,17 +1196,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1501,17 +1517,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F172"/>
+  <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="66" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
@@ -1550,7 +1566,7 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1622,7 +1638,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1639,7 +1655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1656,7 +1672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1673,7 +1689,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1690,7 +1706,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1707,7 +1723,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1724,7 +1740,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1741,7 +1757,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1758,7 +1774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1775,7 +1791,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1792,7 +1808,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1809,7 +1825,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1826,7 +1842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1836,17 +1852,14 @@
       <c r="C19" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
-        <v>367</v>
-      </c>
       <c r="E19" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1863,7 +1876,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1880,7 +1893,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1890,17 +1903,14 @@
       <c r="C22" t="s">
         <v>52</v>
       </c>
-      <c r="D22" t="s">
-        <v>367</v>
-      </c>
       <c r="E22" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1910,17 +1920,14 @@
       <c r="C23" t="s">
         <v>54</v>
       </c>
-      <c r="D23" t="s">
-        <v>367</v>
-      </c>
       <c r="E23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1937,7 +1944,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1954,7 +1961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1964,17 +1971,14 @@
       <c r="C26" t="s">
         <v>60</v>
       </c>
-      <c r="D26" t="s">
-        <v>367</v>
-      </c>
       <c r="E26" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1991,7 +1995,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -2001,17 +2005,14 @@
       <c r="C28" t="s">
         <v>64</v>
       </c>
-      <c r="D28" t="s">
-        <v>367</v>
-      </c>
       <c r="E28" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -2028,7 +2029,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -2072,17 +2073,14 @@
       <c r="C32" t="s">
         <v>72</v>
       </c>
-      <c r="D32" t="s">
-        <v>367</v>
-      </c>
       <c r="E32" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -2092,17 +2090,14 @@
       <c r="C33" t="s">
         <v>74</v>
       </c>
-      <c r="D33" t="s">
-        <v>367</v>
-      </c>
       <c r="E33" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -2115,11 +2110,11 @@
       <c r="E34" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -2136,7 +2131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -2153,7 +2148,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -2170,7 +2165,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -2187,7 +2182,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2204,7 +2199,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -2221,7 +2216,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -2238,7 +2233,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -2255,7 +2250,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>20</v>
       </c>
@@ -2272,7 +2267,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -2289,7 +2284,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>20</v>
       </c>
@@ -2306,7 +2301,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -2316,17 +2311,14 @@
       <c r="C46" t="s">
         <v>100</v>
       </c>
-      <c r="D46" t="s">
-        <v>367</v>
-      </c>
       <c r="E46" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>20</v>
       </c>
@@ -2336,17 +2328,14 @@
       <c r="C47" t="s">
         <v>102</v>
       </c>
-      <c r="D47" t="s">
-        <v>367</v>
-      </c>
       <c r="E47" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>20</v>
       </c>
@@ -2356,17 +2345,14 @@
       <c r="C48" t="s">
         <v>104</v>
       </c>
-      <c r="D48" t="s">
-        <v>367</v>
-      </c>
       <c r="E48" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>20</v>
       </c>
@@ -2393,9 +2379,6 @@
       <c r="C50" t="s">
         <v>108</v>
       </c>
-      <c r="D50" t="s">
-        <v>366</v>
-      </c>
       <c r="E50" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2386,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -2431,7 +2414,7 @@
         <v>112</v>
       </c>
       <c r="D52" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="E52" t="s">
         <v>22</v>
@@ -2440,7 +2423,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>20</v>
       </c>
@@ -2457,7 +2440,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -2474,7 +2457,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -2491,7 +2474,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -2501,17 +2484,14 @@
       <c r="C56" t="s">
         <v>120</v>
       </c>
-      <c r="D56" t="s">
-        <v>367</v>
-      </c>
       <c r="E56" t="s">
         <v>22</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F56" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -2528,7 +2508,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -2545,7 +2525,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -2562,7 +2542,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -2579,7 +2559,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -2596,7 +2576,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -2613,7 +2593,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -2623,17 +2603,14 @@
       <c r="C63" t="s">
         <v>134</v>
       </c>
-      <c r="D63" t="s">
-        <v>367</v>
-      </c>
       <c r="E63" t="s">
         <v>22</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -2650,7 +2627,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -2660,9 +2637,6 @@
       <c r="C65" t="s">
         <v>138</v>
       </c>
-      <c r="D65" t="s">
-        <v>367</v>
-      </c>
       <c r="E65" t="s">
         <v>22</v>
       </c>
@@ -2670,7 +2644,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -2687,7 +2661,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>20</v>
       </c>
@@ -2704,7 +2678,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -2721,7 +2695,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>20</v>
       </c>
@@ -2738,7 +2712,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>20</v>
       </c>
@@ -2755,7 +2729,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>20</v>
       </c>
@@ -2772,7 +2746,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>20</v>
       </c>
@@ -2789,7 +2763,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>20</v>
       </c>
@@ -2806,7 +2780,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>20</v>
       </c>
@@ -2823,7 +2797,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>20</v>
       </c>
@@ -2840,7 +2814,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -2857,7 +2831,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>20</v>
       </c>
@@ -2874,7 +2848,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -2891,7 +2865,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>20</v>
       </c>
@@ -2908,7 +2882,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>20</v>
       </c>
@@ -2925,7 +2899,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>20</v>
       </c>
@@ -2942,7 +2916,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>20</v>
       </c>
@@ -2959,7 +2933,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>20</v>
       </c>
@@ -2976,7 +2950,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -2986,17 +2960,14 @@
       <c r="C84" t="s">
         <v>176</v>
       </c>
-      <c r="D84" t="s">
-        <v>367</v>
-      </c>
       <c r="E84" t="s">
         <v>22</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -3013,7 +2984,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>20</v>
       </c>
@@ -3023,17 +2994,14 @@
       <c r="C86" t="s">
         <v>180</v>
       </c>
-      <c r="D86" t="s">
-        <v>367</v>
-      </c>
       <c r="E86" t="s">
         <v>22</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>20</v>
       </c>
@@ -3050,7 +3018,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>20</v>
       </c>
@@ -3067,7 +3035,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>20</v>
       </c>
@@ -3084,7 +3052,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -3101,7 +3069,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>20</v>
       </c>
@@ -3118,7 +3086,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -3135,7 +3103,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>20</v>
       </c>
@@ -3152,7 +3120,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -3169,7 +3137,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>20</v>
       </c>
@@ -3179,17 +3147,14 @@
       <c r="C95" t="s">
         <v>198</v>
       </c>
-      <c r="D95" t="s">
-        <v>367</v>
-      </c>
       <c r="E95" t="s">
         <v>22</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F95" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>20</v>
       </c>
@@ -3206,7 +3171,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>20</v>
       </c>
@@ -3216,17 +3181,14 @@
       <c r="C97" t="s">
         <v>202</v>
       </c>
-      <c r="D97" t="s">
-        <v>367</v>
-      </c>
       <c r="E97" t="s">
         <v>22</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F97" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>20</v>
       </c>
@@ -3243,7 +3205,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>20</v>
       </c>
@@ -3260,7 +3222,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>20</v>
       </c>
@@ -3277,7 +3239,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>20</v>
       </c>
@@ -3294,7 +3256,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>20</v>
       </c>
@@ -3321,17 +3283,14 @@
       <c r="C103" t="s">
         <v>214</v>
       </c>
-      <c r="D103" t="s">
-        <v>367</v>
-      </c>
       <c r="E103" t="s">
         <v>22</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="F103" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>20</v>
       </c>
@@ -3348,7 +3307,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -3358,17 +3317,14 @@
       <c r="C105" t="s">
         <v>218</v>
       </c>
-      <c r="D105" t="s">
-        <v>367</v>
-      </c>
       <c r="E105" t="s">
         <v>22</v>
       </c>
-      <c r="F105" s="2" t="s">
+      <c r="F105" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>20</v>
       </c>
@@ -3385,7 +3341,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>20</v>
       </c>
@@ -3402,7 +3358,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>20</v>
       </c>
@@ -3419,7 +3375,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>20</v>
       </c>
@@ -3436,7 +3392,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>20</v>
       </c>
@@ -3453,7 +3409,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -3470,7 +3426,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>20</v>
       </c>
@@ -3487,7 +3443,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>20</v>
       </c>
@@ -3504,7 +3460,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>20</v>
       </c>
@@ -3521,7 +3477,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>20</v>
       </c>
@@ -3531,17 +3487,14 @@
       <c r="C115" t="s">
         <v>238</v>
       </c>
-      <c r="D115" t="s">
-        <v>367</v>
-      </c>
       <c r="E115" t="s">
         <v>22</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="F115" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>20</v>
       </c>
@@ -3558,7 +3511,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>20</v>
       </c>
@@ -3575,7 +3528,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>20</v>
       </c>
@@ -3592,7 +3545,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>20</v>
       </c>
@@ -3609,7 +3562,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>20</v>
       </c>
@@ -3626,7 +3579,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>20</v>
       </c>
@@ -3643,7 +3596,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>20</v>
       </c>
@@ -3660,7 +3613,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>20</v>
       </c>
@@ -3677,7 +3630,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>20</v>
       </c>
@@ -3694,7 +3647,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>20</v>
       </c>
@@ -3711,7 +3664,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>20</v>
       </c>
@@ -3728,7 +3681,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>20</v>
       </c>
@@ -3745,7 +3698,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>20</v>
       </c>
@@ -3762,7 +3715,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>20</v>
       </c>
@@ -3779,7 +3732,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>20</v>
       </c>
@@ -3796,7 +3749,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>20</v>
       </c>
@@ -3813,7 +3766,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>20</v>
       </c>
@@ -3830,7 +3783,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>20</v>
       </c>
@@ -3847,7 +3800,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>20</v>
       </c>
@@ -3864,7 +3817,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>20</v>
       </c>
@@ -3881,7 +3834,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>20</v>
       </c>
@@ -3898,7 +3851,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>20</v>
       </c>
@@ -3915,7 +3868,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>20</v>
       </c>
@@ -3925,9 +3878,6 @@
       <c r="C138" t="s">
         <v>284</v>
       </c>
-      <c r="D138" t="s">
-        <v>367</v>
-      </c>
       <c r="E138" t="s">
         <v>22</v>
       </c>
@@ -3935,7 +3885,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>20</v>
       </c>
@@ -3945,17 +3895,14 @@
       <c r="C139" t="s">
         <v>286</v>
       </c>
-      <c r="D139" t="s">
-        <v>367</v>
-      </c>
       <c r="E139" t="s">
         <v>22</v>
       </c>
-      <c r="F139" s="2" t="s">
+      <c r="F139" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>20</v>
       </c>
@@ -3965,17 +3912,14 @@
       <c r="C140" t="s">
         <v>288</v>
       </c>
-      <c r="D140" t="s">
-        <v>367</v>
-      </c>
       <c r="E140" t="s">
         <v>22</v>
       </c>
-      <c r="F140" s="2" t="s">
+      <c r="F140" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>20</v>
       </c>
@@ -3992,572 +3936,648 @@
         <v>291</v>
       </c>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>20</v>
       </c>
       <c r="B142" t="s">
-        <v>293</v>
+        <v>20</v>
       </c>
       <c r="C142" t="s">
         <v>292</v>
       </c>
       <c r="E142" t="s">
+        <v>22</v>
+      </c>
+      <c r="F142" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>20</v>
+      </c>
+      <c r="B143" t="s">
+        <v>20</v>
+      </c>
+      <c r="C143" t="s">
         <v>294</v>
       </c>
-      <c r="F142" t="s">
+      <c r="E143" t="s">
+        <v>22</v>
+      </c>
+      <c r="F143" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A143" t="s">
-        <v>20</v>
-      </c>
-      <c r="B143" t="s">
-        <v>293</v>
-      </c>
-      <c r="C143" t="s">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>20</v>
+      </c>
+      <c r="B144" t="s">
+        <v>20</v>
+      </c>
+      <c r="C144" t="s">
         <v>296</v>
       </c>
-      <c r="E143" t="s">
-        <v>294</v>
-      </c>
-      <c r="F143" t="s">
+      <c r="E144" t="s">
+        <v>22</v>
+      </c>
+      <c r="F144" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A144" t="s">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>20</v>
+      </c>
+      <c r="B145" t="s">
+        <v>20</v>
+      </c>
+      <c r="C145" t="s">
         <v>298</v>
       </c>
-      <c r="B144" t="s">
-        <v>298</v>
-      </c>
-      <c r="C144" t="s">
+      <c r="E145" t="s">
+        <v>22</v>
+      </c>
+      <c r="F145" t="s">
         <v>299</v>
       </c>
-      <c r="E144" t="s">
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>20</v>
+      </c>
+      <c r="B146" t="s">
+        <v>20</v>
+      </c>
+      <c r="C146" t="s">
         <v>300</v>
       </c>
-      <c r="F144" t="s">
+      <c r="E146" t="s">
+        <v>22</v>
+      </c>
+      <c r="F146" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A145" t="s">
-        <v>298</v>
-      </c>
-      <c r="B145" t="s">
-        <v>298</v>
-      </c>
-      <c r="C145" t="s">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>20</v>
+      </c>
+      <c r="B147" t="s">
+        <v>20</v>
+      </c>
+      <c r="C147" t="s">
         <v>302</v>
       </c>
-      <c r="E145" t="s">
-        <v>300</v>
-      </c>
-      <c r="F145" t="s">
+      <c r="E147" t="s">
+        <v>22</v>
+      </c>
+      <c r="F147" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A146" t="s">
-        <v>298</v>
-      </c>
-      <c r="B146" t="s">
-        <v>298</v>
-      </c>
-      <c r="C146" t="s">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>20</v>
+      </c>
+      <c r="B148" t="s">
+        <v>20</v>
+      </c>
+      <c r="C148" t="s">
         <v>304</v>
       </c>
-      <c r="E146" t="s">
-        <v>300</v>
-      </c>
-      <c r="F146" t="s">
+      <c r="E148" t="s">
+        <v>22</v>
+      </c>
+      <c r="F148" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
-        <v>298</v>
-      </c>
-      <c r="B147" t="s">
-        <v>298</v>
-      </c>
-      <c r="C147" t="s">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>20</v>
+      </c>
+      <c r="B149" t="s">
+        <v>20</v>
+      </c>
+      <c r="C149" t="s">
         <v>306</v>
       </c>
-      <c r="E147" t="s">
-        <v>300</v>
-      </c>
-      <c r="F147" t="s">
+      <c r="E149" t="s">
+        <v>22</v>
+      </c>
+      <c r="F149" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A148" t="s">
-        <v>298</v>
-      </c>
-      <c r="B148" t="s">
-        <v>298</v>
-      </c>
-      <c r="C148" t="s">
-        <v>308</v>
-      </c>
-      <c r="E148" t="s">
-        <v>300</v>
-      </c>
-      <c r="F148" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A149" t="s">
-        <v>298</v>
-      </c>
-      <c r="B149" t="s">
-        <v>298</v>
-      </c>
-      <c r="C149" t="s">
-        <v>310</v>
-      </c>
-      <c r="E149" t="s">
-        <v>300</v>
-      </c>
-      <c r="F149" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="B150" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="C150" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E150" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="F150" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="B151" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="C151" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E151" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="F151" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="B152" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="C152" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E152" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="F152" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B153" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C153" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E153" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F153" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
+        <v>308</v>
+      </c>
+      <c r="B154" t="s">
+        <v>308</v>
+      </c>
+      <c r="C154" t="s">
         <v>318</v>
       </c>
-      <c r="B154" t="s">
-        <v>318</v>
-      </c>
-      <c r="C154" t="s">
-        <v>322</v>
-      </c>
       <c r="E154" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F154" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B155" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C155" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E155" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F155" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B156" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C156" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E156" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F156" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B157" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C157" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E157" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F157" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B158" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C158" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E158" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F158" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B159" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="C159" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E159" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="F159" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B160" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C160" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E160" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="F160" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
+        <v>328</v>
+      </c>
+      <c r="B161" t="s">
+        <v>328</v>
+      </c>
+      <c r="C161" t="s">
         <v>334</v>
       </c>
-      <c r="B161" t="s">
-        <v>334</v>
-      </c>
-      <c r="C161" t="s">
-        <v>338</v>
-      </c>
       <c r="E161" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="F161" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B162" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C162" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E162" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="F162" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B163" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C163" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E163" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="F163" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B164" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C164" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E164" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="F164" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B165" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C165" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E165" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="F165" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="B166" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C166" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E166" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="F166" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="B167" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C167" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E167" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="F167" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="B168" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C168" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E168" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="F168" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="B169" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C169" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E169" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="F169" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="B170" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
       <c r="C170" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E170" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="F170" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="B171" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="C171" t="s">
         <v>356</v>
       </c>
       <c r="E171" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="F171" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
+        <v>344</v>
+      </c>
+      <c r="B172" t="s">
+        <v>344</v>
+      </c>
+      <c r="C172" t="s">
+        <v>358</v>
+      </c>
+      <c r="E172" t="s">
+        <v>346</v>
+      </c>
+      <c r="F172" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" t="s">
+        <v>344</v>
+      </c>
+      <c r="C173" t="s">
+        <v>360</v>
+      </c>
+      <c r="E173" t="s">
+        <v>346</v>
+      </c>
+      <c r="F173" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>344</v>
+      </c>
+      <c r="B174" t="s">
+        <v>344</v>
+      </c>
+      <c r="C174" t="s">
         <v>362</v>
       </c>
-      <c r="B172" t="s">
-        <v>362</v>
-      </c>
-      <c r="C172" t="s">
+      <c r="E174" t="s">
+        <v>346</v>
+      </c>
+      <c r="F174" t="s">
         <v>363</v>
       </c>
-      <c r="E172" t="s">
+    </row>
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>344</v>
+      </c>
+      <c r="B175" t="s">
+        <v>344</v>
+      </c>
+      <c r="C175" t="s">
         <v>364</v>
       </c>
-      <c r="F172" t="s">
+      <c r="E175" t="s">
+        <v>346</v>
+      </c>
+      <c r="F175" t="s">
         <v>365</v>
       </c>
     </row>
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>366</v>
+      </c>
+      <c r="B176" t="s">
+        <v>367</v>
+      </c>
+      <c r="C176" t="s">
+        <v>367</v>
+      </c>
+      <c r="E176" t="s">
+        <v>368</v>
+      </c>
+      <c r="F176" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>366</v>
+      </c>
+      <c r="B177" t="s">
+        <v>366</v>
+      </c>
+      <c r="C177" t="s">
+        <v>366</v>
+      </c>
+      <c r="E177" t="s">
+        <v>370</v>
+      </c>
+      <c r="F177" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>372</v>
+      </c>
+      <c r="B178" t="s">
+        <v>372</v>
+      </c>
+      <c r="C178" t="s">
+        <v>373</v>
+      </c>
+      <c r="E178" t="s">
+        <v>374</v>
+      </c>
+      <c r="F178" t="s">
+        <v>375</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F172" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
+  <autoFilter ref="A1:F178" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="Yes"/>
+        <filter val="ADAS_PG_SYS_RM"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="D2:D172" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D178" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="F47" r:id="rId1" xr:uid="{D18D7C4D-33C2-4B80-BA7A-BD15EBA3FD8A}"/>
-    <hyperlink ref="F48" r:id="rId2" xr:uid="{84675358-2A08-416F-AE55-CFB2CAC22526}"/>
-    <hyperlink ref="F46" r:id="rId3" xr:uid="{BF5EEDA7-6029-4478-BF15-F327605970ED}"/>
-    <hyperlink ref="F2" r:id="rId4" xr:uid="{385F474B-64B7-44FD-B019-ADFF124A53A6}"/>
-    <hyperlink ref="F139" r:id="rId5" xr:uid="{47FBD93F-1084-4488-9F1D-B487000C81CF}"/>
-    <hyperlink ref="F140" r:id="rId6" xr:uid="{F9DF473E-A37E-4F8F-831D-74DB3BB64708}"/>
-    <hyperlink ref="F19" r:id="rId7" xr:uid="{53DEA8FE-EA42-4C16-B9BD-ECC612BE8548}"/>
-    <hyperlink ref="F22" r:id="rId8" xr:uid="{DFDD021F-0E7E-4EC1-9C34-F7508C593A99}"/>
-    <hyperlink ref="F23" r:id="rId9" xr:uid="{F8000198-1375-4056-B8B0-F062D6CA35AD}"/>
-    <hyperlink ref="F32" r:id="rId10" xr:uid="{7124F89C-CD3A-4D72-9E45-A27D310E528C}"/>
-    <hyperlink ref="F33" r:id="rId11" xr:uid="{6DB75DA6-FF08-4CA1-9E34-67541823D270}"/>
-    <hyperlink ref="F34" r:id="rId12" xr:uid="{60BE7B1D-E8C1-4468-80EE-898A63165000}"/>
-    <hyperlink ref="F26" r:id="rId13" xr:uid="{7BC996E1-B491-46A2-8870-2F5827809AAD}"/>
-    <hyperlink ref="F28" r:id="rId14" xr:uid="{B215E829-5D4A-4D3A-BF70-1272003BE6E6}"/>
-    <hyperlink ref="F56" r:id="rId15" xr:uid="{C1CCCA3F-5C64-49F8-95DA-EC7F3AF540E3}"/>
-    <hyperlink ref="F63" r:id="rId16" xr:uid="{7F119410-33AD-499B-B7D4-BE1C34A55E23}"/>
-    <hyperlink ref="F84" r:id="rId17" xr:uid="{E93E5E27-8549-4788-B83A-281DD1416E8E}"/>
-    <hyperlink ref="F86" r:id="rId18" xr:uid="{2B3C2462-74A5-429E-BD2F-C96FB6473624}"/>
-    <hyperlink ref="F95" r:id="rId19" xr:uid="{7610388B-F166-474B-8BBB-172B3214156F}"/>
-    <hyperlink ref="F97" r:id="rId20" xr:uid="{0256E75A-1753-4B0A-B675-75B3FF4C127C}"/>
-    <hyperlink ref="F105" r:id="rId21" xr:uid="{CC93E6DB-86AE-49FA-A194-94EE5A67A7A1}"/>
-    <hyperlink ref="F115" r:id="rId22" xr:uid="{2FB3AEE1-59DA-4087-B35F-F09DBA0B18A6}"/>
-    <hyperlink ref="F103" r:id="rId23" xr:uid="{E68933AC-BB4F-42C1-8514-B17D1659C5C2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>